<commit_message>
finalize data driven testing
</commit_message>
<xml_diff>
--- a/HelloDDT/testData/caldata2.xlsx
+++ b/HelloDDT/testData/caldata2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SeleniumPractice\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Initial Deposit amout</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -96,7 +102,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +119,26 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -154,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -174,6 +200,11 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,14 +493,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="31.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="18.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="24.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="34.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="7" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="14.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="10.85546875" collapsed="true"/>
+    <col min="8" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -514,7 +545,9 @@
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" t="s" s="9">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
@@ -535,7 +568,9 @@
       <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" t="s" s="10">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
@@ -556,7 +591,9 @@
       <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" t="s" s="11">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
@@ -577,7 +614,9 @@
       <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" t="s" s="12">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
@@ -598,7 +637,9 @@
       <c r="F6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" t="s" s="13">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>